<commit_message>
actualizando excel de datos y componiendo el codigo para que agarre toda las columnas que se deseen agreagar
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\UVG-MM2021-Crecimiento-Poblacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306600A7-A5F4-4201-BC3D-1FC3F24E4650}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230D93E5-C8C1-41B7-8D52-147E023B0BF6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -315,8 +315,8 @@
   </sheetPr>
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -350,7 +350,9 @@
       <c r="C2" s="3">
         <v>1650</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3">
+        <v>4000</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -362,7 +364,9 @@
       <c r="C3" s="3">
         <v>1658</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3">
+        <v>4019</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -374,7 +378,9 @@
       <c r="C4" s="3">
         <v>1666</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>4039</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -386,7 +392,9 @@
       <c r="C5" s="3">
         <v>1674</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>4058</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -398,7 +406,9 @@
       <c r="C6" s="3">
         <v>1682</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>4078</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -410,7 +420,9 @@
       <c r="C7" s="3">
         <v>1690</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3">
+        <v>4097</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -422,7 +434,9 @@
       <c r="C8" s="3">
         <v>1698</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3">
+        <v>4117</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -434,7 +448,9 @@
       <c r="C9" s="3">
         <v>1706</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3">
+        <v>4136</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -446,7 +462,9 @@
       <c r="C10" s="3">
         <v>1714</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3">
+        <v>4156</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -458,7 +476,9 @@
       <c r="C11" s="3">
         <v>1722</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3">
+        <v>4175</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -470,7 +490,9 @@
       <c r="C12" s="3">
         <v>1730</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3">
+        <v>4194</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -482,7 +504,9 @@
       <c r="C13" s="3">
         <v>1738</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3">
+        <v>4214</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -494,7 +518,9 @@
       <c r="C14" s="3">
         <v>1746</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3">
+        <v>4233</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -506,7 +532,9 @@
       <c r="C15" s="3">
         <v>1754</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3">
+        <v>4253</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -518,7 +546,9 @@
       <c r="C16" s="3">
         <v>1762</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3">
+        <v>4272</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -530,7 +560,9 @@
       <c r="C17" s="3">
         <v>1770</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3">
+        <v>4292</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -542,7 +574,9 @@
       <c r="C18" s="3">
         <v>1779</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3">
+        <v>4312</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -554,7 +588,9 @@
       <c r="C19" s="3">
         <v>1788</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3">
+        <v>4335</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -566,7 +602,9 @@
       <c r="C20" s="3">
         <v>1798</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3">
+        <v>4358</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -578,7 +616,9 @@
       <c r="C21" s="3">
         <v>1808</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3">
+        <v>4383</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -590,7 +630,9 @@
       <c r="C22" s="3">
         <v>1819</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3">
+        <v>4410</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -602,7 +644,9 @@
       <c r="C23" s="3">
         <v>1830</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3">
+        <v>4437</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -614,7 +658,9 @@
       <c r="C24" s="3">
         <v>1842</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3">
+        <v>4466</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -626,7 +672,9 @@
       <c r="C25" s="3">
         <v>1855</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3">
+        <v>4497</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -638,7 +686,9 @@
       <c r="C26" s="3">
         <v>1868</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3">
+        <v>4529</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -650,7 +700,9 @@
       <c r="C27" s="3">
         <v>1882</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3">
+        <v>4562</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
@@ -662,7 +714,9 @@
       <c r="C28" s="3">
         <v>1896</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3">
+        <v>4597</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
@@ -674,7 +728,9 @@
       <c r="C29" s="3">
         <v>1911</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="3">
+        <v>4633</v>
+      </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -686,7 +742,9 @@
       <c r="C30" s="3">
         <v>1926</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3">
+        <v>4670</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -698,7 +756,9 @@
       <c r="C31" s="3">
         <v>1942</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3">
+        <v>4709</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -710,7 +770,9 @@
       <c r="C32" s="3">
         <v>1959</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3">
+        <v>4749</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -722,7 +784,9 @@
       <c r="C33" s="3">
         <v>1976</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3">
+        <v>4791</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
@@ -734,7 +798,9 @@
       <c r="C34" s="3">
         <v>1994</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3">
+        <v>4834</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -746,7 +812,9 @@
       <c r="C35" s="3">
         <v>2013</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="3">
+        <v>4879</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
@@ -758,7 +826,9 @@
       <c r="C36" s="3">
         <v>2032</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3">
+        <v>4926</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
@@ -770,7 +840,9 @@
       <c r="C37" s="3">
         <v>2051</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3">
+        <v>4973</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -782,7 +854,9 @@
       <c r="C38" s="3">
         <v>2071</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3">
+        <v>5020</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
@@ -794,7 +868,9 @@
       <c r="C39" s="3">
         <v>2081</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3">
+        <v>5069</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
@@ -806,7 +882,9 @@
       <c r="C40" s="3">
         <v>2111</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3">
+        <v>5118</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
@@ -818,7 +896,9 @@
       <c r="C41" s="3">
         <v>2132</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3">
+        <v>5168</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
@@ -830,7 +910,9 @@
       <c r="C42" s="3">
         <v>2153</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="3">
+        <v>5219</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
@@ -842,7 +924,9 @@
       <c r="C43" s="3">
         <v>2175</v>
       </c>
-      <c r="D43" s="3"/>
+      <c r="D43" s="3">
+        <v>5272</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
@@ -854,7 +938,9 @@
       <c r="C44" s="3">
         <v>2197</v>
       </c>
-      <c r="D44" s="3"/>
+      <c r="D44" s="3">
+        <v>5325</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
@@ -866,7 +952,9 @@
       <c r="C45" s="3">
         <v>2219</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="3">
+        <v>5380</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
@@ -878,7 +966,9 @@
       <c r="C46" s="3">
         <v>2242</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="3">
+        <v>5436</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
@@ -890,7 +980,9 @@
       <c r="C47" s="3">
         <v>2266</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3">
+        <v>5493</v>
+      </c>
     </row>
     <row r="48" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
@@ -902,7 +994,9 @@
       <c r="C48" s="3">
         <v>2290</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="3">
+        <v>5552</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
@@ -914,7 +1008,9 @@
       <c r="C49" s="3">
         <v>2315</v>
       </c>
-      <c r="D49" s="3"/>
+      <c r="D49" s="3">
+        <v>5613</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
@@ -926,7 +1022,9 @@
       <c r="C50" s="3">
         <v>2341</v>
       </c>
-      <c r="D50" s="3"/>
+      <c r="D50" s="3">
+        <v>5675</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
@@ -938,7 +1036,9 @@
       <c r="C51" s="3">
         <v>2368</v>
       </c>
-      <c r="D51" s="3"/>
+      <c r="D51" s="3">
+        <v>5740</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
@@ -950,7 +1050,9 @@
       <c r="C52" s="3">
         <v>2395</v>
       </c>
-      <c r="D52" s="3"/>
+      <c r="D52" s="3">
+        <v>5806</v>
+      </c>
     </row>
     <row r="53" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
@@ -962,7 +1064,9 @@
       <c r="C53" s="3">
         <v>2423</v>
       </c>
-      <c r="D53" s="3"/>
+      <c r="D53" s="3">
+        <v>5874</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
@@ -974,7 +1078,9 @@
       <c r="C54" s="3">
         <v>2452</v>
       </c>
-      <c r="D54" s="3"/>
+      <c r="D54" s="3">
+        <v>5944</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
@@ -986,7 +1092,9 @@
       <c r="C55" s="3">
         <v>2482</v>
       </c>
-      <c r="D55" s="3"/>
+      <c r="D55" s="3">
+        <v>6016</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
@@ -998,7 +1106,9 @@
       <c r="C56" s="3">
         <v>2512</v>
       </c>
-      <c r="D56" s="3"/>
+      <c r="D56" s="3">
+        <v>6089</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
@@ -1010,7 +1120,9 @@
       <c r="C57" s="3">
         <v>2543</v>
       </c>
-      <c r="D57" s="3"/>
+      <c r="D57" s="3">
+        <v>6164</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
@@ -1022,7 +1134,9 @@
       <c r="C58" s="3">
         <v>2574</v>
       </c>
-      <c r="D58" s="3"/>
+      <c r="D58" s="3">
+        <v>6241</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
@@ -1034,7 +1148,9 @@
       <c r="C59" s="3">
         <v>2607</v>
       </c>
-      <c r="D59" s="3"/>
+      <c r="D59" s="3">
+        <v>6319</v>
+      </c>
     </row>
     <row r="60" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
@@ -1046,7 +1162,9 @@
       <c r="C60" s="3">
         <v>2640</v>
       </c>
-      <c r="D60" s="3"/>
+      <c r="D60" s="3">
+        <v>6399</v>
+      </c>
     </row>
     <row r="61" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
@@ -1058,7 +1176,9 @@
       <c r="C61" s="3">
         <v>2673</v>
       </c>
-      <c r="D61" s="3"/>
+      <c r="D61" s="3">
+        <v>6481</v>
+      </c>
     </row>
     <row r="62" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
@@ -1070,7 +1190,9 @@
       <c r="C62" s="3">
         <v>2708</v>
       </c>
-      <c r="D62" s="3"/>
+      <c r="D62" s="3">
+        <v>6564</v>
+      </c>
     </row>
     <row r="63" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
@@ -1082,7 +1204,9 @@
       <c r="C63" s="3">
         <v>2743</v>
       </c>
-      <c r="D63" s="3"/>
+      <c r="D63" s="3">
+        <v>6649</v>
+      </c>
     </row>
     <row r="64" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
@@ -1094,7 +1218,9 @@
       <c r="C64" s="3">
         <v>2778</v>
       </c>
-      <c r="D64" s="3"/>
+      <c r="D64" s="3">
+        <v>6735</v>
+      </c>
     </row>
     <row r="65" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
@@ -1106,7 +1232,9 @@
       <c r="C65" s="3">
         <v>2815</v>
       </c>
-      <c r="D65" s="3"/>
+      <c r="D65" s="3">
+        <v>6823</v>
+      </c>
     </row>
     <row r="66" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
@@ -1118,7 +1246,9 @@
       <c r="C66" s="3">
         <v>2852</v>
       </c>
-      <c r="D66" s="3"/>
+      <c r="D66" s="3">
+        <v>6913</v>
+      </c>
     </row>
     <row r="67" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
@@ -1130,7 +1260,9 @@
       <c r="C67" s="3">
         <v>2889</v>
       </c>
-      <c r="D67" s="3"/>
+      <c r="D67" s="3">
+        <v>7004</v>
+      </c>
     </row>
     <row r="68" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
@@ -1142,7 +1274,9 @@
       <c r="C68" s="3">
         <v>2928</v>
       </c>
-      <c r="D68" s="3"/>
+      <c r="D68" s="3">
+        <v>7098</v>
+      </c>
     </row>
     <row r="69" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
@@ -1154,7 +1288,9 @@
       <c r="C69" s="3">
         <v>2967</v>
       </c>
-      <c r="D69" s="3"/>
+      <c r="D69" s="3">
+        <v>7193</v>
+      </c>
     </row>
     <row r="70" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
@@ -1166,7 +1302,9 @@
       <c r="C70" s="3">
         <v>3007</v>
       </c>
-      <c r="D70" s="3"/>
+      <c r="D70" s="3">
+        <v>7290</v>
+      </c>
     </row>
     <row r="71" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
@@ -1178,7 +1316,9 @@
       <c r="C71" s="3">
         <v>3048</v>
       </c>
-      <c r="D71" s="3"/>
+      <c r="D71" s="3">
+        <v>7389</v>
+      </c>
     </row>
     <row r="72" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
@@ -1190,7 +1330,9 @@
       <c r="C72" s="3">
         <v>3089</v>
       </c>
-      <c r="D72" s="3"/>
+      <c r="D72" s="3">
+        <v>7489</v>
+      </c>
     </row>
     <row r="73" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
@@ -1202,7 +1344,9 @@
       <c r="C73" s="3">
         <v>3132</v>
       </c>
-      <c r="D73" s="3"/>
+      <c r="D73" s="3">
+        <v>7592</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
@@ -1214,7 +1358,9 @@
       <c r="C74" s="3">
         <v>3175</v>
       </c>
-      <c r="D74" s="3"/>
+      <c r="D74" s="3">
+        <v>7697</v>
+      </c>
     </row>
     <row r="75" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
@@ -1226,7 +1372,9 @@
       <c r="C75" s="3">
         <v>3211</v>
       </c>
-      <c r="D75" s="3"/>
+      <c r="D75" s="3">
+        <v>7784</v>
+      </c>
     </row>
     <row r="76" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
@@ -1238,7 +1386,9 @@
       <c r="C76" s="3">
         <v>3248</v>
       </c>
-      <c r="D76" s="3"/>
+      <c r="D76" s="3">
+        <v>7874</v>
+      </c>
     </row>
     <row r="77" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
@@ -1250,7 +1400,9 @@
       <c r="C77" s="3">
         <v>3286</v>
       </c>
-      <c r="D77" s="3"/>
+      <c r="D77" s="3">
+        <v>7966</v>
+      </c>
     </row>
     <row r="78" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
@@ -1262,7 +1414,9 @@
       <c r="C78" s="3">
         <v>3325</v>
       </c>
-      <c r="D78" s="3"/>
+      <c r="D78" s="3">
+        <v>8060</v>
+      </c>
     </row>
     <row r="79" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
@@ -1274,7 +1428,9 @@
       <c r="C79" s="3">
         <v>3364</v>
       </c>
-      <c r="D79" s="3"/>
+      <c r="D79" s="3">
+        <v>8156</v>
+      </c>
     </row>
     <row r="80" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
@@ -1286,7 +1442,9 @@
       <c r="C80" s="3">
         <v>3405</v>
       </c>
-      <c r="D80" s="3"/>
+      <c r="D80" s="3">
+        <v>8255</v>
+      </c>
     </row>
     <row r="81" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
@@ -1298,7 +1456,9 @@
       <c r="C81" s="3">
         <v>3447</v>
       </c>
-      <c r="D81" s="3"/>
+      <c r="D81" s="3">
+        <v>8356</v>
+      </c>
     </row>
     <row r="82" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
@@ -1310,7 +1470,9 @@
       <c r="C82" s="3">
         <v>3489</v>
       </c>
-      <c r="D82" s="3"/>
+      <c r="D82" s="3">
+        <v>8459</v>
+      </c>
     </row>
     <row r="83" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
@@ -1322,7 +1484,9 @@
       <c r="C83" s="3">
         <v>3533</v>
       </c>
-      <c r="D83" s="3"/>
+      <c r="D83" s="3">
+        <v>8564</v>
+      </c>
     </row>
     <row r="84" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
@@ -1334,7 +1498,9 @@
       <c r="C84" s="3">
         <v>3577</v>
       </c>
-      <c r="D84" s="3"/>
+      <c r="D84" s="3">
+        <v>8672</v>
+      </c>
     </row>
     <row r="85" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
@@ -1346,7 +1512,9 @@
       <c r="C85" s="3">
         <v>3623</v>
       </c>
-      <c r="D85" s="3"/>
+      <c r="D85" s="3">
+        <v>8782</v>
+      </c>
     </row>
     <row r="86" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
@@ -1358,7 +1526,9 @@
       <c r="C86" s="3">
         <v>3669</v>
       </c>
-      <c r="D86" s="3"/>
+      <c r="D86" s="3">
+        <v>8895</v>
+      </c>
     </row>
     <row r="87" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
@@ -1370,7 +1540,9 @@
       <c r="C87" s="3">
         <v>3716</v>
       </c>
-      <c r="D87" s="3"/>
+      <c r="D87" s="3">
+        <v>9009</v>
+      </c>
     </row>
     <row r="88" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
@@ -1382,7 +1554,9 @@
       <c r="C88" s="3">
         <v>3765</v>
       </c>
-      <c r="D88" s="3"/>
+      <c r="D88" s="3">
+        <v>9127</v>
+      </c>
     </row>
     <row r="89" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
@@ -1394,7 +1568,9 @@
       <c r="C89" s="3">
         <v>3814</v>
       </c>
-      <c r="D89" s="3"/>
+      <c r="D89" s="3">
+        <v>9246</v>
+      </c>
     </row>
     <row r="90" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
@@ -1406,7 +1582,9 @@
       <c r="C90" s="3">
         <v>3864</v>
       </c>
-      <c r="D90" s="3"/>
+      <c r="D90" s="3">
+        <v>9366</v>
+      </c>
     </row>
     <row r="91" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
@@ -1418,7 +1596,9 @@
       <c r="C91" s="3">
         <v>3914</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3">
+        <v>9488</v>
+      </c>
     </row>
     <row r="92" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
@@ -1430,7 +1610,9 @@
       <c r="C92" s="3">
         <v>3964</v>
       </c>
-      <c r="D92" s="3"/>
+      <c r="D92" s="3">
+        <v>9610</v>
+      </c>
     </row>
     <row r="93" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
@@ -1442,7 +1624,9 @@
       <c r="C93" s="3">
         <v>4015</v>
       </c>
-      <c r="D93" s="3"/>
+      <c r="D93" s="3">
+        <v>9734</v>
+      </c>
     </row>
     <row r="94" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
@@ -1454,7 +1638,9 @@
       <c r="C94" s="3">
         <v>4067</v>
       </c>
-      <c r="D94" s="3"/>
+      <c r="D94" s="3">
+        <v>9859</v>
+      </c>
     </row>
     <row r="95" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
@@ -1466,7 +1652,9 @@
       <c r="C95" s="3">
         <v>4119</v>
       </c>
-      <c r="D95" s="3"/>
+      <c r="D95" s="3">
+        <v>9985</v>
+      </c>
     </row>
     <row r="96" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
@@ -1478,7 +1666,9 @@
       <c r="C96" s="3">
         <v>4171</v>
       </c>
-      <c r="D96" s="3"/>
+      <c r="D96" s="3">
+        <v>10112</v>
+      </c>
     </row>
     <row r="97" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
@@ -1490,7 +1680,9 @@
       <c r="C97" s="3">
         <v>4224</v>
       </c>
-      <c r="D97" s="3"/>
+      <c r="D97" s="3">
+        <v>10241</v>
+      </c>
     </row>
     <row r="98" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
@@ -1502,7 +1694,9 @@
       <c r="C98" s="3">
         <v>4278</v>
       </c>
-      <c r="D98" s="3"/>
+      <c r="D98" s="3">
+        <v>10371</v>
+      </c>
     </row>
     <row r="99" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
@@ -1514,7 +1708,9 @@
       <c r="C99" s="3">
         <v>4332</v>
       </c>
-      <c r="D99" s="3"/>
+      <c r="D99" s="3">
+        <v>10502</v>
+      </c>
     </row>
     <row r="100" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
@@ -1526,7 +1722,9 @@
       <c r="C100" s="3">
         <v>4387</v>
       </c>
-      <c r="D100" s="3"/>
+      <c r="D100" s="3">
+        <v>10635</v>
+      </c>
     </row>
     <row r="101" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
@@ -1538,7 +1736,9 @@
       <c r="C101" s="3">
         <v>4442</v>
       </c>
-      <c r="D101" s="3"/>
+      <c r="D101" s="3">
+        <v>10769</v>
+      </c>
     </row>
     <row r="102" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
@@ -1550,7 +1750,9 @@
       <c r="C102" s="3">
         <v>4498</v>
       </c>
-      <c r="D102" s="3"/>
+      <c r="D102" s="3">
+        <v>10905</v>
+      </c>
     </row>
     <row r="103" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
@@ -1562,7 +1764,9 @@
       <c r="C103" s="3">
         <v>4555</v>
       </c>
-      <c r="D103" s="3"/>
+      <c r="D103" s="3">
+        <v>11043</v>
+      </c>
     </row>
     <row r="104" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
@@ -1574,7 +1778,9 @@
       <c r="C104" s="3">
         <v>4612</v>
       </c>
-      <c r="D104" s="3"/>
+      <c r="D104" s="3">
+        <v>11182</v>
+      </c>
     </row>
     <row r="105" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
@@ -1586,7 +1792,9 @@
       <c r="C105" s="3">
         <v>4670</v>
       </c>
-      <c r="D105" s="3"/>
+      <c r="D105" s="3">
+        <v>11322</v>
+      </c>
     </row>
     <row r="106" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
@@ -1598,7 +1806,9 @@
       <c r="C106" s="3">
         <v>4729</v>
       </c>
-      <c r="D106" s="3"/>
+      <c r="D106" s="3">
+        <v>11464</v>
+      </c>
     </row>
     <row r="107" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
@@ -1610,7 +1820,9 @@
       <c r="C107" s="3">
         <v>4788</v>
       </c>
-      <c r="D107" s="3"/>
+      <c r="D107" s="3">
+        <v>11608</v>
+      </c>
     </row>
     <row r="108" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
@@ -1622,7 +1834,9 @@
       <c r="C108" s="3">
         <v>4848</v>
       </c>
-      <c r="D108" s="3"/>
+      <c r="D108" s="3">
+        <v>11752</v>
+      </c>
     </row>
     <row r="109" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
@@ -1634,7 +1848,9 @@
       <c r="C109" s="3">
         <v>4909</v>
       </c>
-      <c r="D109" s="3"/>
+      <c r="D109" s="3">
+        <v>11900</v>
+      </c>
     </row>
     <row r="110" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
@@ -1646,7 +1862,9 @@
       <c r="C110" s="3">
         <v>4971</v>
       </c>
-      <c r="D110" s="3"/>
+      <c r="D110" s="3">
+        <v>12050</v>
+      </c>
     </row>
     <row r="111" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
@@ -1658,7 +1876,9 @@
       <c r="C111" s="3">
         <v>5033</v>
       </c>
-      <c r="D111" s="3"/>
+      <c r="D111" s="3">
+        <v>12202</v>
+      </c>
     </row>
     <row r="112" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
@@ -1670,7 +1890,9 @@
       <c r="C112" s="3">
         <v>5097</v>
       </c>
-      <c r="D112" s="3"/>
+      <c r="D112" s="3">
+        <v>12357</v>
+      </c>
     </row>
     <row r="113" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
@@ -1682,7 +1904,9 @@
       <c r="C113" s="3">
         <v>5162</v>
       </c>
-      <c r="D113" s="3"/>
+      <c r="D113" s="3">
+        <v>12515</v>
+      </c>
     </row>
     <row r="114" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
@@ -1694,7 +1918,9 @@
       <c r="C114" s="3">
         <v>5228</v>
       </c>
-      <c r="D114" s="3"/>
+      <c r="D114" s="3">
+        <v>12674</v>
+      </c>
     </row>
     <row r="115" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
@@ -1706,7 +1932,9 @@
       <c r="C115" s="3">
         <v>5295</v>
       </c>
-      <c r="D115" s="3"/>
+      <c r="D115" s="3">
+        <v>12836</v>
+      </c>
     </row>
     <row r="116" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
@@ -1718,7 +1946,9 @@
       <c r="C116" s="3">
         <v>5363</v>
       </c>
-      <c r="D116" s="3"/>
+      <c r="D116" s="3">
+        <v>13001</v>
+      </c>
     </row>
     <row r="117" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
@@ -1730,7 +1960,9 @@
       <c r="C117" s="3">
         <v>5431</v>
       </c>
-      <c r="D117" s="3"/>
+      <c r="D117" s="3">
+        <v>13167</v>
+      </c>
     </row>
     <row r="118" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
@@ -1742,7 +1974,9 @@
       <c r="C118" s="3">
         <v>5501</v>
       </c>
-      <c r="D118" s="3"/>
+      <c r="D118" s="3">
+        <v>13335</v>
+      </c>
     </row>
     <row r="119" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
@@ -1754,7 +1988,9 @@
       <c r="C119" s="3">
         <v>5571</v>
       </c>
-      <c r="D119" s="3"/>
+      <c r="D119" s="3">
+        <v>13506</v>
+      </c>
     </row>
     <row r="120" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
@@ -1766,7 +2002,9 @@
       <c r="C120" s="3">
         <v>5642</v>
       </c>
-      <c r="D120" s="3"/>
+      <c r="D120" s="3">
+        <v>13678</v>
+      </c>
     </row>
     <row r="121" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
@@ -1778,7 +2016,9 @@
       <c r="C121" s="3">
         <v>5714</v>
       </c>
-      <c r="D121" s="3"/>
+      <c r="D121" s="3">
+        <v>13853</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>